<commit_message>
added plotting func to fb scraper
</commit_message>
<xml_diff>
--- a/CCScraper_2/results.xlsx
+++ b/CCScraper_2/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,545 +453,413 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SkyProductserviceSkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
+          <t>Sky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sky</t>
+          <t>sky tv</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SkyProductserviceSkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
+          <t>Sky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SkyProductservice</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
+          <t>Sky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SkyProductservice</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow groupSee allPagesSkyProductservice  1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
+          <t>Sky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SkyProductservice</t>
+          <t>Sky TV    Follow      Shared with PublicThe Last of Us has been an emotional rollercoaster</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
+          <t>Sky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SkyProductservice</t>
+          <t>Sky TV Sky Showcase  Sky Documentaries and Now TVWith Repeats on Sky Documentaries on Sun 5th at 710pm Tuesday 7th  9pm Friday 10th  1050pm Saturday 11th  5pm000  000FRZ2duNORW</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sky Sports</t>
+          <t>Sky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SkyProductservice</t>
+          <t>Sky TV    Follow      Shared with PublicSuns out guns out</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sky Sports</t>
+          <t>Sky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SkyProductservice</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sky Sports</t>
+          <t>Sky TV Channel</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SkyProductservice</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow groupSee allPagesSkyProductservice  1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sky Sports</t>
+          <t>Sky TV Channel</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SkyProductservice</t>
+          <t>Sky TV    Follow      Shared with PublicThe Last of Us has been an emotional rollercoaster</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SkyTV channel</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sky Sports</t>
+          <t>Sky TV Channel</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky TV Sky Showcase  Sky Documentaries and Now TVWith Repeats on Sky Documentaries on Sun 5th at 710pm Tuesday 7th  9pm Friday 10th  1050pm Saturday 11th  5pm000  000FRZ2duNORW</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like thisFollowSky Sports FootballTV channel  1</t>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoinSky TV ChannelPublic  311 following  2 posts a weekThis is the official youtube channel of Sky TV</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
+          <t>Sky TV Channel</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky TV    Follow      Shared with PublicSuns out guns out</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like thisFollowSky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
-        </is>
-      </c>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoin</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like thisFollowSky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
-        </is>
-      </c>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoin</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow groupSee allPagesSkyProductservice  1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like thisFollowSky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
-        </is>
-      </c>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoin</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky TV    Follow      Shared with PublicThe Last of Us has been an emotional rollercoaster</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like thisFollowSky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
-        </is>
-      </c>
+          <t>SKY TVPrivate  355 membersWe Promote LegacyJoin</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky TV Sky Showcase  Sky Documentaries and Now TVWith Repeats on Sky Documentaries on Sun 5th at 710pm Tuesday 7th  9pm Friday 10th  1050pm Saturday 11th  5pm000  000FRZ2duNORW</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like thisFollow</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
-        </is>
-      </c>
+          <t>SKY TVPrivate  355 membersWe Promote Legacy</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TV    Follow      Shared with PublicSuns out guns out</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like thisFollow</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Sky Sports Football our new page for the beautiful game</t>
-        </is>
-      </c>
+          <t>SKY TVPrivate  355 membersWe Promote Legacy</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like thisFollow</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Sky Sports Football</t>
-        </is>
-      </c>
+          <t>SKY TVPrivate  355 membersWe Promote Legacy</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow groupSee allPagesSkyProductservice  1</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like thisFollow</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Sky Sports Football</t>
-        </is>
-      </c>
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TV    Follow      Shared with PublicThe Last of Us has been an emotional rollercoaster</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on FacebookMuhammad Abdullahi and 45 other friends like this</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Sky Sports Football</t>
-        </is>
-      </c>
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TV Sky Showcase  Sky Documentaries and Now TVWith Repeats on Sky Documentaries on Sun 5th at 710pm Tuesday 7th  9pm Friday 10th  1050pm Saturday 11th  5pm000  000FRZ2duNORW</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on Facebook</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Sky Sports Football</t>
-        </is>
-      </c>
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TV    Follow      Shared with PublicSuns out guns out</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Sky SportsTV network  12M likes  10 posts in the last 2 weeksThe home of Sky Sports on Facebook</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Sky Sports Football</t>
-        </is>
-      </c>
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Sky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Sky Sports Football UpdatesPrivate  138K members  10 posts a dayJoin</t>
-        </is>
-      </c>
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow groupSee allPagesSkyProductservice  1</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Sky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Sky Sports Football UpdatesPrivate  138K members  10 posts a dayJoin</t>
-        </is>
-      </c>
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TV    Follow      Shared with PublicThe Last of Us has been an emotional rollercoaster</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Sky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Sky Sports Football UpdatesPrivate  138K members  10 posts a dayJoin</t>
-        </is>
-      </c>
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TV Sky Showcase  Sky Documentaries and Now TVWith Repeats on Sky Documentaries on Sun 5th at 710pm Tuesday 7th  9pm Friday 10th  1050pm Saturday 11th  5pm000  000FRZ2duNORW</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Sky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Sky Sports Football UpdatesPrivate  138K members  10 posts a dayJoin</t>
-        </is>
-      </c>
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TV    Follow      Shared with PublicSuns out guns out</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Sky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Sky Sports Football UpdatesPrivate  138K members  10 posts a day</t>
-        </is>
-      </c>
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Sky  Visual Arts  5 out of 5  79K likes  10 posts in the last 2 weeksDISCLAIMER We hereby declare that we do not own the rights to the music and videos used in the background</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Sky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Sky Sports Football UpdatesPrivate  138K members  10 posts a day</t>
-        </is>
-      </c>
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow groupSee allPagesSkyProductservice  1</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Sky Sports FootballTV channel  1</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Sky Sports Football UpdatesPrivate  138K members  10 posts a day</t>
-        </is>
-      </c>
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky TV    Follow      Shared with PublicThe Last of Us has been an emotional rollercoaster</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Sky Sports Football Updates</t>
-        </is>
-      </c>
+      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky TV Sky Showcase  Sky Documentaries and Now TVWith Repeats on Sky Documentaries on Sun 5th at 710pm Tuesday 7th  9pm Friday 10th  1050pm Saturday 11th  5pm000  000FRZ2duNORW</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Sky Sports Football Updates</t>
-        </is>
-      </c>
+      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Sky</t>
+          <t>Sky TV    Follow      Shared with PublicSuns out guns out</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Sky Sports Football Updates</t>
-        </is>
-      </c>
+      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>SkySport_NewsPublic  36K following  2 posts a daySavaging of top English Spanish Italian German and French teamsFollow group</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Sky Sports Football Updates</t>
-        </is>
-      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SkySport_NewsPublic  36K following  2 posts a daySavaging of top English Spanish Italian German and French teamsFollow group</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1000,7 +868,7 @@
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>SkySport_NewsPublic  36K following  2 posts a daySavaging of top English Spanish Italian German and French teamsFollow group</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1009,7 +877,7 @@
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>SkySport_NewsPublic  36K following  2 posts a daySavaging of top English Spanish Italian German and French teamsFollow group</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1018,7 +886,7 @@
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SkySport_NewsPublic  36K following  2 posts a daySavaging of top English Spanish Italian German and French teams</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1027,7 +895,7 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SkySport_NewsPublic  36K following  2 posts a daySavaging of top English Spanish Italian German and French teams</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1036,7 +904,7 @@
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SkySport_NewsPublic  36K following  2 posts a daySavaging of top English Spanish Italian German and French teams</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1045,7 +913,7 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SkySport_News</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1054,7 +922,7 @@
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SkySport_News</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1063,7 +931,7 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SkySport_News</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1072,7 +940,7 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SkySport_News</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1081,7 +949,7 @@
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friendsMessageŚkÿ WåłkęřFriend17 mutual friendsMessageChukwunoyerem Bethel Bïl SkyDigital creator  4</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1090,7 +958,7 @@
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friendsMessageŚkÿ WåłkęřFriend17 mutual friendsMessageChukwunoyerem Bethel Bïl SkyDigital creator  4</t>
+          <t>Sky TVTV network   1</t>
         </is>
       </c>
     </row>
@@ -1099,7 +967,7 @@
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friendsMessageŚkÿ WåłkęřFriend17 mutual friendsMessageChukwunoyerem Bethel Bïl SkyDigital creator  4</t>
+          <t>Sky TV</t>
         </is>
       </c>
     </row>
@@ -1108,7 +976,7 @@
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friendsMessageŚkÿ WåłkęřFriend17 mutual friendsMessageChukwunoyerem Bethel Bïl SkyDigital creator  4</t>
+          <t>Sky TV</t>
         </is>
       </c>
     </row>
@@ -1117,7 +985,7 @@
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friendsMessageŚkÿ WåłkęřFriend17 mutual friendsMessageChukwunoyerem Bethel Bïl SkyDigital creator  4</t>
+          <t>Sky TV</t>
         </is>
       </c>
     </row>
@@ -1126,7 +994,7 @@
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friendsMessage</t>
+          <t>Sky TV</t>
         </is>
       </c>
     </row>
@@ -1135,7 +1003,7 @@
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friendsMessage</t>
+          <t>Sky TV</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1012,7 @@
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friendsMessage</t>
+          <t>Sky TV</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1021,7 @@
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friendsMessage</t>
+          <t>Sky TV</t>
         </is>
       </c>
     </row>
@@ -1162,7 +1030,7 @@
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Sky ManFriend4 mutual friends</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow group</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1039,7 @@
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Sky ManFriend</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow group</t>
         </is>
       </c>
     </row>
@@ -1180,7 +1048,7 @@
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Sky ManFriend</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow group</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1057,7 @@
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Sky Man</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow group</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1066,7 @@
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Sky Man</t>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow group</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1075,7 @@
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Sky Man</t>
+          <t>SKY TV</t>
         </is>
       </c>
     </row>
@@ -1216,7 +1084,358 @@
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Sky Man</t>
+          <t>SKY TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>SKY TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>SKY TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow group</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow group</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow group</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Sky tvPublic  356 following  8 posts a yearFollow group</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Sky tvPublic  356 following  8 posts a year</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Sky tvPublic  356 following  8 posts a year</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Sky tvPublic  356 following  8 posts a year</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Sky tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Sky tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Sky tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Sky tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow      Shared with Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow      Shared with Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow      Shared with Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow      Shared with Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow      Shared with Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow      Shared with Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow      Shared with Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow      Shared with Public</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Sky TV    Follow</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Sky TV</t>
         </is>
       </c>
     </row>

</xml_diff>